<commit_message>
got lat longs for Elahi
</commit_message>
<xml_diff>
--- a/sbs_meta/output/sbs_meta.xlsx
+++ b/sbs_meta/output/sbs_meta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38680" yWindow="6000" windowWidth="26440" windowHeight="10660" tabRatio="500"/>
+    <workbookView xWindow="4480" yWindow="3100" windowWidth="21460" windowHeight="9440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="study_table" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>entered_by</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>n_comparisons</t>
+  </si>
+  <si>
+    <t>hadLong</t>
+  </si>
+  <si>
+    <t>hadLat</t>
+  </si>
+  <si>
+    <t>hadYear1</t>
+  </si>
+  <si>
+    <t>hadYear2</t>
   </si>
 </sst>
 </file>
@@ -242,8 +254,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -295,7 +323,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +344,14 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +372,14 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,11 +709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -679,15 +723,16 @@
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="42.5" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="9" width="9.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="42.5" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="16" thickBot="1">
+    <row r="1" spans="1:34" ht="16" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -704,24 +749,32 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -738,8 +791,12 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:34">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -755,23 +812,36 @@
       <c r="E2" s="1">
         <v>33.555</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>-117.824</v>
+      </c>
+      <c r="G2" s="1">
+        <v>33.542000000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <f>1869 - 10</f>
+        <v>1859</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2001</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1">
+      <c r="K2" s="1">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="L2" s="1">
         <v>3</v>
       </c>
-      <c r="I2" s="1">
+      <c r="M2" s="1">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:34">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -787,23 +857,36 @@
       <c r="E3" s="1">
         <v>44.255000000000003</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>-68.385000000000005</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44.234000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <f>1915-10</f>
+        <v>1905</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2007</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="1">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="1">
+      <c r="M3" s="1">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:34">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -813,16 +896,35 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>-121.9049</v>
+      </c>
+      <c r="E4" s="1">
+        <v>36.621859999999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-121.895</v>
+      </c>
+      <c r="G4" s="1">
+        <v>36.628999999999998</v>
+      </c>
+      <c r="H4" s="1">
+        <f xml:space="preserve"> 1947 - 10</f>
+        <v>1937</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2015</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1">
+      <c r="K4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="L4" s="1">
         <v>2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="M4" s="1">
         <v>10</v>
       </c>
     </row>

</xml_diff>